<commit_message>
Update during 2024 Progress
</commit_message>
<xml_diff>
--- a/03 Parameter Estimation/experimental_data/tracer_1.xlsx
+++ b/03 Parameter Estimation/experimental_data/tracer_1.xlsx
@@ -450,7 +450,7 @@
         <v>0</v>
       </c>
       <c r="B2" t="n">
-        <v>0.0008440804018733693</v>
+        <v>0.0006129782144667135</v>
       </c>
     </row>
     <row r="3">
@@ -458,7 +458,7 @@
         <v>0.5</v>
       </c>
       <c r="B3" t="n">
-        <v>0.0005177679613787094</v>
+        <v>0.000167030288430012</v>
       </c>
     </row>
     <row r="4">
@@ -466,7 +466,7 @@
         <v>1</v>
       </c>
       <c r="B4" t="n">
-        <v>-0.0001132690555414689</v>
+        <v>0.0004338922338852587</v>
       </c>
     </row>
     <row r="5">
@@ -474,7 +474,7 @@
         <v>1.5</v>
       </c>
       <c r="B5" t="n">
-        <v>-0.0005861986554842646</v>
+        <v>-0.0002170762416254172</v>
       </c>
     </row>
     <row r="6">
@@ -482,7 +482,7 @@
         <v>2</v>
       </c>
       <c r="B6" t="n">
-        <v>0.0008703225791384605</v>
+        <v>0.0008747278146306797</v>
       </c>
     </row>
     <row r="7">
@@ -490,7 +490,7 @@
         <v>2.5</v>
       </c>
       <c r="B7" t="n">
-        <v>-0.0004892050782420588</v>
+        <v>0.0007321593349610904</v>
       </c>
     </row>
     <row r="8">
@@ -498,7 +498,7 @@
         <v>3</v>
       </c>
       <c r="B8" t="n">
-        <v>-0.0003916057689362943</v>
+        <v>-0.0004941261119279359</v>
       </c>
     </row>
     <row r="9">
@@ -506,7 +506,7 @@
         <v>3.5</v>
       </c>
       <c r="B9" t="n">
-        <v>-0.0007489057732223397</v>
+        <v>0.0006767489191618478</v>
       </c>
     </row>
     <row r="10">
@@ -514,7 +514,7 @@
         <v>4</v>
       </c>
       <c r="B10" t="n">
-        <v>0.0007731403995436434</v>
+        <v>0.0001793662792943235</v>
       </c>
     </row>
     <row r="11">
@@ -522,7 +522,7 @@
         <v>4.5</v>
       </c>
       <c r="B11" t="n">
-        <v>0.0006511697742613872</v>
+        <v>0.000870476746643765</v>
       </c>
     </row>
     <row r="12">
@@ -530,7 +530,7 @@
         <v>5</v>
       </c>
       <c r="B12" t="n">
-        <v>0.0003651213337376964</v>
+        <v>0.0003596577860992075</v>
       </c>
     </row>
     <row r="13">
@@ -538,7 +538,7 @@
         <v>5.5</v>
       </c>
       <c r="B13" t="n">
-        <v>-0.0006186168033105032</v>
+        <v>-0.0004171409912206486</v>
       </c>
     </row>
     <row r="14">
@@ -546,7 +546,7 @@
         <v>6</v>
       </c>
       <c r="B14" t="n">
-        <v>5.253451168644388e-05</v>
+        <v>-0.0005654394159180649</v>
       </c>
     </row>
     <row r="15">
@@ -554,7 +554,7 @@
         <v>6.5</v>
       </c>
       <c r="B15" t="n">
-        <v>-0.0008197441789647599</v>
+        <v>8.060235797638928e-05</v>
       </c>
     </row>
     <row r="16">
@@ -562,7 +562,7 @@
         <v>7</v>
       </c>
       <c r="B16" t="n">
-        <v>-0.0004026169245616225</v>
+        <v>-0.0008682207403359941</v>
       </c>
     </row>
     <row r="17">
@@ -570,7 +570,7 @@
         <v>7.5</v>
       </c>
       <c r="B17" t="n">
-        <v>-0.00054687030898172</v>
+        <v>-0.0002887339829283358</v>
       </c>
     </row>
     <row r="18">
@@ -578,7 +578,7 @@
         <v>8</v>
       </c>
       <c r="B18" t="n">
-        <v>0.0004488092339587279</v>
+        <v>0.0008721298224477597</v>
       </c>
     </row>
     <row r="19">
@@ -586,7 +586,7 @@
         <v>8.5</v>
       </c>
       <c r="B19" t="n">
-        <v>0.0003186850410849701</v>
+        <v>-0.0006428465687840929</v>
       </c>
     </row>
     <row r="20">
@@ -594,7 +594,7 @@
         <v>9</v>
       </c>
       <c r="B20" t="n">
-        <v>-0.0005402359334698348</v>
+        <v>-7.902698040923016e-05</v>
       </c>
     </row>
     <row r="21">
@@ -602,7 +602,7 @@
         <v>9.5</v>
       </c>
       <c r="B21" t="n">
-        <v>-0.0004019527567478386</v>
+        <v>0.0004292929352018653</v>
       </c>
     </row>
     <row r="22">
@@ -610,7 +610,7 @@
         <v>10</v>
       </c>
       <c r="B22" t="n">
-        <v>-0.0001878694630511251</v>
+        <v>-2.094558717066373e-05</v>
       </c>
     </row>
     <row r="23">
@@ -618,7 +618,7 @@
         <v>10.5</v>
       </c>
       <c r="B23" t="n">
-        <v>0.0008024430293258894</v>
+        <v>0.0006391408394164846</v>
       </c>
     </row>
     <row r="24">
@@ -626,7 +626,7 @@
         <v>11</v>
       </c>
       <c r="B24" t="n">
-        <v>0.0001117439494907421</v>
+        <v>0.0003455314566379251</v>
       </c>
     </row>
     <row r="25">
@@ -634,7 +634,7 @@
         <v>11.5</v>
       </c>
       <c r="B25" t="n">
-        <v>0.000836188349101943</v>
+        <v>-4.971380381298716e-05</v>
       </c>
     </row>
     <row r="26">
@@ -642,7 +642,7 @@
         <v>12</v>
       </c>
       <c r="B26" t="n">
-        <v>0.0006549858096795542</v>
+        <v>0.0007534094984500119</v>
       </c>
     </row>
     <row r="27">
@@ -650,7 +650,7 @@
         <v>12.5</v>
       </c>
       <c r="B27" t="n">
-        <v>-0.0005009080918855084</v>
+        <v>2.12486176405015e-06</v>
       </c>
     </row>
     <row r="28">
@@ -658,7 +658,7 @@
         <v>13</v>
       </c>
       <c r="B28" t="n">
-        <v>-0.0001424414191764569</v>
+        <v>-4.362381800764414e-05</v>
       </c>
     </row>
     <row r="29">
@@ -666,7 +666,7 @@
         <v>13.5</v>
       </c>
       <c r="B29" t="n">
-        <v>-2.324163373035838e-05</v>
+        <v>0.0007399577365479697</v>
       </c>
     </row>
     <row r="30">
@@ -674,7 +674,7 @@
         <v>14</v>
       </c>
       <c r="B30" t="n">
-        <v>-6.656714232984833e-05</v>
+        <v>0.0005713046302452364</v>
       </c>
     </row>
     <row r="31">
@@ -682,7 +682,7 @@
         <v>14.5</v>
       </c>
       <c r="B31" t="n">
-        <v>0.0007875340960348577</v>
+        <v>0.0004442982179013407</v>
       </c>
     </row>
     <row r="32">
@@ -690,7 +690,7 @@
         <v>15</v>
       </c>
       <c r="B32" t="n">
-        <v>0.0005556683708605656</v>
+        <v>0.000679639669131734</v>
       </c>
     </row>
     <row r="33">
@@ -698,7 +698,7 @@
         <v>15.5</v>
       </c>
       <c r="B33" t="n">
-        <v>0.001848170155002429</v>
+        <v>0.001159129464333824</v>
       </c>
     </row>
     <row r="34">
@@ -706,7 +706,7 @@
         <v>16</v>
       </c>
       <c r="B34" t="n">
-        <v>0.002355011644951486</v>
+        <v>0.001791187463929095</v>
       </c>
     </row>
     <row r="35">
@@ -714,7 +714,7 @@
         <v>16.5</v>
       </c>
       <c r="B35" t="n">
-        <v>0.002081173837187266</v>
+        <v>0.002721119299695902</v>
       </c>
     </row>
     <row r="36">
@@ -722,7 +722,7 @@
         <v>17</v>
       </c>
       <c r="B36" t="n">
-        <v>0.00320948790809555</v>
+        <v>0.00270877505582611</v>
       </c>
     </row>
     <row r="37">
@@ -730,7 +730,7 @@
         <v>17.5</v>
       </c>
       <c r="B37" t="n">
-        <v>0.004977466791897592</v>
+        <v>0.003942462291944053</v>
       </c>
     </row>
     <row r="38">
@@ -738,7 +738,7 @@
         <v>18</v>
       </c>
       <c r="B38" t="n">
-        <v>0.00542853549729872</v>
+        <v>0.006258298773560275</v>
       </c>
     </row>
     <row r="39">
@@ -746,7 +746,7 @@
         <v>18.5</v>
       </c>
       <c r="B39" t="n">
-        <v>0.007300831212725245</v>
+        <v>0.0068439514944732</v>
       </c>
     </row>
     <row r="40">
@@ -754,7 +754,7 @@
         <v>19</v>
       </c>
       <c r="B40" t="n">
-        <v>0.008159059499796182</v>
+        <v>0.007174606663179334</v>
       </c>
     </row>
     <row r="41">
@@ -762,7 +762,7 @@
         <v>19.5</v>
       </c>
       <c r="B41" t="n">
-        <v>0.009338239514843411</v>
+        <v>0.009845449035499424</v>
       </c>
     </row>
     <row r="42">
@@ -770,7 +770,7 @@
         <v>20</v>
       </c>
       <c r="B42" t="n">
-        <v>0.01137131032174985</v>
+        <v>0.01165362221613702</v>
       </c>
     </row>
     <row r="43">
@@ -778,7 +778,7 @@
         <v>20.5</v>
       </c>
       <c r="B43" t="n">
-        <v>0.01173559212613833</v>
+        <v>0.01265623823682351</v>
       </c>
     </row>
     <row r="44">
@@ -786,7 +786,7 @@
         <v>21</v>
       </c>
       <c r="B44" t="n">
-        <v>0.01509791528711685</v>
+        <v>0.01413474277444923</v>
       </c>
     </row>
     <row r="45">
@@ -794,7 +794,7 @@
         <v>21.5</v>
       </c>
       <c r="B45" t="n">
-        <v>0.01649042909686012</v>
+        <v>0.01643313091262052</v>
       </c>
     </row>
     <row r="46">
@@ -802,7 +802,7 @@
         <v>22</v>
       </c>
       <c r="B46" t="n">
-        <v>0.01782145369976416</v>
+        <v>0.01827563346399179</v>
       </c>
     </row>
     <row r="47">
@@ -810,7 +810,7 @@
         <v>22.5</v>
       </c>
       <c r="B47" t="n">
-        <v>0.01855339190137763</v>
+        <v>0.01847872851662083</v>
       </c>
     </row>
     <row r="48">
@@ -818,7 +818,7 @@
         <v>23</v>
       </c>
       <c r="B48" t="n">
-        <v>0.02037962881739914</v>
+        <v>0.02144875408940707</v>
       </c>
     </row>
     <row r="49">
@@ -826,7 +826,7 @@
         <v>23.5</v>
       </c>
       <c r="B49" t="n">
-        <v>0.02301289554396982</v>
+        <v>0.02167083917188617</v>
       </c>
     </row>
     <row r="50">
@@ -834,7 +834,7 @@
         <v>24</v>
       </c>
       <c r="B50" t="n">
-        <v>0.02322288541749219</v>
+        <v>0.02344332619257251</v>
       </c>
     </row>
     <row r="51">
@@ -842,7 +842,7 @@
         <v>24.5</v>
       </c>
       <c r="B51" t="n">
-        <v>0.02521877750479968</v>
+        <v>0.02448212489602493</v>
       </c>
     </row>
     <row r="52">
@@ -850,7 +850,7 @@
         <v>25</v>
       </c>
       <c r="B52" t="n">
-        <v>0.02620734899734882</v>
+        <v>0.02671295951740811</v>
       </c>
     </row>
     <row r="53">
@@ -858,7 +858,7 @@
         <v>25.5</v>
       </c>
       <c r="B53" t="n">
-        <v>0.02708195252491182</v>
+        <v>0.02867426288683521</v>
       </c>
     </row>
     <row r="54">
@@ -866,7 +866,7 @@
         <v>26</v>
       </c>
       <c r="B54" t="n">
-        <v>0.028854104767128</v>
+        <v>0.02846431888518712</v>
       </c>
     </row>
     <row r="55">
@@ -874,7 +874,7 @@
         <v>26.5</v>
       </c>
       <c r="B55" t="n">
-        <v>0.03053723643655392</v>
+        <v>0.03041498145802725</v>
       </c>
     </row>
     <row r="56">
@@ -882,7 +882,7 @@
         <v>27</v>
       </c>
       <c r="B56" t="n">
-        <v>0.03154495990575502</v>
+        <v>0.03096024575413269</v>
       </c>
     </row>
     <row r="57">
@@ -890,7 +890,7 @@
         <v>27.5</v>
       </c>
       <c r="B57" t="n">
-        <v>0.03148358444846442</v>
+        <v>0.03145508832977217</v>
       </c>
     </row>
     <row r="58">
@@ -898,7 +898,7 @@
         <v>28</v>
       </c>
       <c r="B58" t="n">
-        <v>0.03352344658285396</v>
+        <v>0.03289776998073373</v>
       </c>
     </row>
     <row r="59">
@@ -906,7 +906,7 @@
         <v>28.5</v>
       </c>
       <c r="B59" t="n">
-        <v>0.0326152327796071</v>
+        <v>0.03293906435107861</v>
       </c>
     </row>
     <row r="60">
@@ -914,7 +914,7 @@
         <v>29</v>
       </c>
       <c r="B60" t="n">
-        <v>0.03315076786670422</v>
+        <v>0.0341264445964834</v>
       </c>
     </row>
     <row r="61">
@@ -922,7 +922,7 @@
         <v>29.5</v>
       </c>
       <c r="B61" t="n">
-        <v>0.03375058859781019</v>
+        <v>0.03364946797660232</v>
       </c>
     </row>
     <row r="62">
@@ -930,7 +930,7 @@
         <v>30</v>
       </c>
       <c r="B62" t="n">
-        <v>0.03542811845872364</v>
+        <v>0.03535365191816073</v>
       </c>
     </row>
     <row r="63">
@@ -938,7 +938,7 @@
         <v>30.5</v>
       </c>
       <c r="B63" t="n">
-        <v>0.03522731269523575</v>
+        <v>0.03515876065363194</v>
       </c>
     </row>
     <row r="64">
@@ -946,7 +946,7 @@
         <v>31</v>
       </c>
       <c r="B64" t="n">
-        <v>0.03550091464193553</v>
+        <v>0.03584743254506771</v>
       </c>
     </row>
     <row r="65">
@@ -954,7 +954,7 @@
         <v>31.5</v>
       </c>
       <c r="B65" t="n">
-        <v>0.0356258776971172</v>
+        <v>0.03469969066104423</v>
       </c>
     </row>
     <row r="66">
@@ -962,7 +962,7 @@
         <v>32</v>
       </c>
       <c r="B66" t="n">
-        <v>0.0350300117461406</v>
+        <v>0.03455071102079953</v>
       </c>
     </row>
     <row r="67">
@@ -970,7 +970,7 @@
         <v>32.5</v>
       </c>
       <c r="B67" t="n">
-        <v>0.03478358108591405</v>
+        <v>0.03449536887988677</v>
       </c>
     </row>
     <row r="68">
@@ -978,7 +978,7 @@
         <v>33</v>
       </c>
       <c r="B68" t="n">
-        <v>0.03398700313317982</v>
+        <v>0.03532342011401784</v>
       </c>
     </row>
     <row r="69">
@@ -986,7 +986,7 @@
         <v>33.5</v>
       </c>
       <c r="B69" t="n">
-        <v>0.03426488953672085</v>
+        <v>0.03456242667364493</v>
       </c>
     </row>
     <row r="70">
@@ -994,7 +994,7 @@
         <v>34</v>
       </c>
       <c r="B70" t="n">
-        <v>0.03432835571256116</v>
+        <v>0.03435129138349304</v>
       </c>
     </row>
     <row r="71">
@@ -1002,7 +1002,7 @@
         <v>34.5</v>
       </c>
       <c r="B71" t="n">
-        <v>0.03371595994793785</v>
+        <v>0.03352621119474267</v>
       </c>
     </row>
     <row r="72">
@@ -1010,7 +1010,7 @@
         <v>35</v>
       </c>
       <c r="B72" t="n">
-        <v>0.03420043893023161</v>
+        <v>0.03372504613429261</v>
       </c>
     </row>
     <row r="73">
@@ -1018,7 +1018,7 @@
         <v>35.5</v>
       </c>
       <c r="B73" t="n">
-        <v>0.03363099062897489</v>
+        <v>0.0334851326522166</v>
       </c>
     </row>
     <row r="74">
@@ -1026,7 +1026,7 @@
         <v>36</v>
       </c>
       <c r="B74" t="n">
-        <v>0.03227038950663509</v>
+        <v>0.0326885813559009</v>
       </c>
     </row>
     <row r="75">
@@ -1034,7 +1034,7 @@
         <v>36.5</v>
       </c>
       <c r="B75" t="n">
-        <v>0.03291023475473208</v>
+        <v>0.03207781505707574</v>
       </c>
     </row>
     <row r="76">
@@ -1042,7 +1042,7 @@
         <v>37</v>
       </c>
       <c r="B76" t="n">
-        <v>0.03158811652684839</v>
+        <v>0.03202652464374498</v>
       </c>
     </row>
     <row r="77">
@@ -1050,7 +1050,7 @@
         <v>37.5</v>
       </c>
       <c r="B77" t="n">
-        <v>0.03096685593090327</v>
+        <v>0.03139907975954529</v>
       </c>
     </row>
     <row r="78">
@@ -1058,7 +1058,7 @@
         <v>38</v>
       </c>
       <c r="B78" t="n">
-        <v>0.03102565872961855</v>
+        <v>0.03028148297702781</v>
       </c>
     </row>
     <row r="79">
@@ -1066,7 +1066,7 @@
         <v>38.5</v>
       </c>
       <c r="B79" t="n">
-        <v>0.03010587890904979</v>
+        <v>0.02973022336123666</v>
       </c>
     </row>
     <row r="80">
@@ -1074,7 +1074,7 @@
         <v>39</v>
       </c>
       <c r="B80" t="n">
-        <v>0.02959053112629101</v>
+        <v>0.02947438928417772</v>
       </c>
     </row>
     <row r="81">
@@ -1082,7 +1082,7 @@
         <v>39.5</v>
       </c>
       <c r="B81" t="n">
-        <v>0.0280625578435591</v>
+        <v>0.02842494819879137</v>
       </c>
     </row>
     <row r="82">
@@ -1090,7 +1090,7 @@
         <v>40</v>
       </c>
       <c r="B82" t="n">
-        <v>0.02722930287297007</v>
+        <v>0.02847928785185023</v>
       </c>
     </row>
     <row r="83">
@@ -1098,7 +1098,7 @@
         <v>40.5</v>
       </c>
       <c r="B83" t="n">
-        <v>0.02648208545568187</v>
+        <v>0.02729220625081223</v>
       </c>
     </row>
     <row r="84">
@@ -1106,7 +1106,7 @@
         <v>41</v>
       </c>
       <c r="B84" t="n">
-        <v>0.02557161499808533</v>
+        <v>0.02684376286519028</v>
       </c>
     </row>
     <row r="85">
@@ -1114,7 +1114,7 @@
         <v>41.5</v>
       </c>
       <c r="B85" t="n">
-        <v>0.0250441380715518</v>
+        <v>0.02612414455941189</v>
       </c>
     </row>
     <row r="86">
@@ -1122,7 +1122,7 @@
         <v>42</v>
       </c>
       <c r="B86" t="n">
-        <v>0.02543364846557387</v>
+        <v>0.02549170123640418</v>
       </c>
     </row>
     <row r="87">
@@ -1130,7 +1130,7 @@
         <v>42.5</v>
       </c>
       <c r="B87" t="n">
-        <v>0.02359026476856222</v>
+        <v>0.02354264694082608</v>
       </c>
     </row>
     <row r="88">
@@ -1138,7 +1138,7 @@
         <v>43</v>
       </c>
       <c r="B88" t="n">
-        <v>0.02325746446906702</v>
+        <v>0.02382327851564674</v>
       </c>
     </row>
     <row r="89">
@@ -1146,7 +1146,7 @@
         <v>43.5</v>
       </c>
       <c r="B89" t="n">
-        <v>0.02304229742183351</v>
+        <v>0.02229562870847374</v>
       </c>
     </row>
     <row r="90">
@@ -1154,7 +1154,7 @@
         <v>44</v>
       </c>
       <c r="B90" t="n">
-        <v>0.02298533299889812</v>
+        <v>0.02256618554451306</v>
       </c>
     </row>
     <row r="91">
@@ -1162,7 +1162,7 @@
         <v>44.5</v>
       </c>
       <c r="B91" t="n">
-        <v>0.02219371664162221</v>
+        <v>0.02223810225210569</v>
       </c>
     </row>
     <row r="92">
@@ -1170,7 +1170,7 @@
         <v>45</v>
       </c>
       <c r="B92" t="n">
-        <v>0.02169977884015573</v>
+        <v>0.02147683531516774</v>
       </c>
     </row>
     <row r="93">
@@ -1178,7 +1178,7 @@
         <v>45.5</v>
       </c>
       <c r="B93" t="n">
-        <v>0.02081705394960589</v>
+        <v>0.02040955525337468</v>
       </c>
     </row>
     <row r="94">
@@ -1186,7 +1186,7 @@
         <v>46</v>
       </c>
       <c r="B94" t="n">
-        <v>0.02041244859055625</v>
+        <v>0.01956961754315481</v>
       </c>
     </row>
     <row r="95">
@@ -1194,7 +1194,7 @@
         <v>46.5</v>
       </c>
       <c r="B95" t="n">
-        <v>0.01888747201509037</v>
+        <v>0.01951359856292885</v>
       </c>
     </row>
     <row r="96">
@@ -1202,7 +1202,7 @@
         <v>47</v>
       </c>
       <c r="B96" t="n">
-        <v>0.01785134635550895</v>
+        <v>0.01913291085668976</v>
       </c>
     </row>
     <row r="97">
@@ -1210,7 +1210,7 @@
         <v>47.5</v>
       </c>
       <c r="B97" t="n">
-        <v>0.01722701695415134</v>
+        <v>0.01718622513026559</v>
       </c>
     </row>
     <row r="98">
@@ -1218,7 +1218,7 @@
         <v>48</v>
       </c>
       <c r="B98" t="n">
-        <v>0.01666260587992424</v>
+        <v>0.01794673400769296</v>
       </c>
     </row>
     <row r="99">
@@ -1226,7 +1226,7 @@
         <v>48.5</v>
       </c>
       <c r="B99" t="n">
-        <v>0.01626029782098945</v>
+        <v>0.01593092866812602</v>
       </c>
     </row>
     <row r="100">
@@ -1234,7 +1234,7 @@
         <v>49</v>
       </c>
       <c r="B100" t="n">
-        <v>0.01535302389508347</v>
+        <v>0.01577149069930894</v>
       </c>
     </row>
     <row r="101">
@@ -1242,7 +1242,7 @@
         <v>49.5</v>
       </c>
       <c r="B101" t="n">
-        <v>0.0158577518149928</v>
+        <v>0.01506045832126794</v>
       </c>
     </row>
     <row r="102">
@@ -1250,7 +1250,7 @@
         <v>50</v>
       </c>
       <c r="B102" t="n">
-        <v>0.014091228944705</v>
+        <v>0.01492273975108071</v>
       </c>
     </row>
     <row r="103">
@@ -1258,7 +1258,7 @@
         <v>50.5</v>
       </c>
       <c r="B103" t="n">
-        <v>0.01382631532963034</v>
+        <v>0.01405858238032199</v>
       </c>
     </row>
     <row r="104">
@@ -1266,7 +1266,7 @@
         <v>51</v>
       </c>
       <c r="B104" t="n">
-        <v>0.01383591597962585</v>
+        <v>0.01439230522799444</v>
       </c>
     </row>
     <row r="105">
@@ -1274,7 +1274,7 @@
         <v>51.5</v>
       </c>
       <c r="B105" t="n">
-        <v>0.01316973010780545</v>
+        <v>0.01404634903871807</v>
       </c>
     </row>
     <row r="106">
@@ -1282,7 +1282,7 @@
         <v>52</v>
       </c>
       <c r="B106" t="n">
-        <v>0.01310976124837276</v>
+        <v>0.0132265947550028</v>
       </c>
     </row>
     <row r="107">
@@ -1290,7 +1290,7 @@
         <v>52.5</v>
       </c>
       <c r="B107" t="n">
-        <v>0.01163038815956492</v>
+        <v>0.01259802624399598</v>
       </c>
     </row>
     <row r="108">
@@ -1298,7 +1298,7 @@
         <v>53</v>
       </c>
       <c r="B108" t="n">
-        <v>0.0126090372029591</v>
+        <v>0.01241988781316653</v>
       </c>
     </row>
     <row r="109">
@@ -1306,7 +1306,7 @@
         <v>53.5</v>
       </c>
       <c r="B109" t="n">
-        <v>0.01162427673393152</v>
+        <v>0.01178856334425026</v>
       </c>
     </row>
     <row r="110">
@@ -1314,7 +1314,7 @@
         <v>54</v>
       </c>
       <c r="B110" t="n">
-        <v>0.01180510050141457</v>
+        <v>0.01177387336657145</v>
       </c>
     </row>
     <row r="111">
@@ -1322,7 +1322,7 @@
         <v>54.5</v>
       </c>
       <c r="B111" t="n">
-        <v>0.0112855901416639</v>
+        <v>0.01057857908867601</v>
       </c>
     </row>
     <row r="112">
@@ -1330,7 +1330,7 @@
         <v>55</v>
       </c>
       <c r="B112" t="n">
-        <v>0.01075319919123812</v>
+        <v>0.01102081536996148</v>
       </c>
     </row>
     <row r="113">
@@ -1338,7 +1338,7 @@
         <v>55.5</v>
       </c>
       <c r="B113" t="n">
-        <v>0.01022858028924534</v>
+        <v>0.009018171912452877</v>
       </c>
     </row>
     <row r="114">
@@ -1346,7 +1346,7 @@
         <v>56</v>
       </c>
       <c r="B114" t="n">
-        <v>0.01027523713223078</v>
+        <v>0.009813177877154402</v>
       </c>
     </row>
     <row r="115">
@@ -1354,7 +1354,7 @@
         <v>56.5</v>
       </c>
       <c r="B115" t="n">
-        <v>0.009248944983374125</v>
+        <v>0.009611711766524573</v>
       </c>
     </row>
     <row r="116">
@@ -1362,7 +1362,7 @@
         <v>57</v>
       </c>
       <c r="B116" t="n">
-        <v>0.008208560508476547</v>
+        <v>0.008715411567699921</v>
       </c>
     </row>
     <row r="117">
@@ -1370,7 +1370,7 @@
         <v>57.5</v>
       </c>
       <c r="B117" t="n">
-        <v>0.008535345044322396</v>
+        <v>0.008327027958035887</v>
       </c>
     </row>
     <row r="118">
@@ -1378,7 +1378,7 @@
         <v>58</v>
       </c>
       <c r="B118" t="n">
-        <v>0.008038311781768006</v>
+        <v>0.008698477671879659</v>
       </c>
     </row>
     <row r="119">
@@ -1386,7 +1386,7 @@
         <v>58.5</v>
       </c>
       <c r="B119" t="n">
-        <v>0.00815218991032666</v>
+        <v>0.007717442921966847</v>
       </c>
     </row>
     <row r="120">
@@ -1394,7 +1394,7 @@
         <v>59</v>
       </c>
       <c r="B120" t="n">
-        <v>0.00674042896293657</v>
+        <v>0.00728759285058629</v>
       </c>
     </row>
     <row r="121">
@@ -1402,7 +1402,7 @@
         <v>59.5</v>
       </c>
       <c r="B121" t="n">
-        <v>0.006978798609167642</v>
+        <v>0.006503019149229266</v>
       </c>
     </row>
     <row r="122">
@@ -1410,7 +1410,7 @@
         <v>60</v>
       </c>
       <c r="B122" t="n">
-        <v>0.00637621295181885</v>
+        <v>0.006461873295517968</v>
       </c>
     </row>
     <row r="123">
@@ -1418,7 +1418,7 @@
         <v>60.5</v>
       </c>
       <c r="B123" t="n">
-        <v>0.006136636382195015</v>
+        <v>0.00723346083177696</v>
       </c>
     </row>
     <row r="124">
@@ -1426,7 +1426,7 @@
         <v>61</v>
       </c>
       <c r="B124" t="n">
-        <v>0.005861496448046168</v>
+        <v>0.006225862615475493</v>
       </c>
     </row>
     <row r="125">
@@ -1434,7 +1434,7 @@
         <v>61.5</v>
       </c>
       <c r="B125" t="n">
-        <v>0.006644016789219489</v>
+        <v>0.006413358539882419</v>
       </c>
     </row>
     <row r="126">
@@ -1442,7 +1442,7 @@
         <v>62</v>
       </c>
       <c r="B126" t="n">
-        <v>0.005159807391720165</v>
+        <v>0.006219340183987928</v>
       </c>
     </row>
     <row r="127">
@@ -1450,7 +1450,7 @@
         <v>62.5</v>
       </c>
       <c r="B127" t="n">
-        <v>0.005207109362754403</v>
+        <v>0.004975768058713966</v>
       </c>
     </row>
     <row r="128">
@@ -1458,7 +1458,7 @@
         <v>63</v>
       </c>
       <c r="B128" t="n">
-        <v>0.00583910717593882</v>
+        <v>0.005272875115562521</v>
       </c>
     </row>
     <row r="129">
@@ -1466,7 +1466,7 @@
         <v>63.5</v>
       </c>
       <c r="B129" t="n">
-        <v>0.004422953215510981</v>
+        <v>0.004408934151144996</v>
       </c>
     </row>
     <row r="130">
@@ -1474,7 +1474,7 @@
         <v>64</v>
       </c>
       <c r="B130" t="n">
-        <v>0.005327432452862768</v>
+        <v>0.004996407338401098</v>
       </c>
     </row>
     <row r="131">
@@ -1482,7 +1482,7 @@
         <v>64.5</v>
       </c>
       <c r="B131" t="n">
-        <v>0.004968237593556431</v>
+        <v>0.003827601234203077</v>
       </c>
     </row>
     <row r="132">
@@ -1490,7 +1490,7 @@
         <v>65</v>
       </c>
       <c r="B132" t="n">
-        <v>0.005227781558357666</v>
+        <v>0.00521668267688786</v>
       </c>
     </row>
     <row r="133">
@@ -1498,7 +1498,7 @@
         <v>65.5</v>
       </c>
       <c r="B133" t="n">
-        <v>0.004575970416917502</v>
+        <v>0.003788762635288112</v>
       </c>
     </row>
     <row r="134">
@@ -1506,7 +1506,7 @@
         <v>66</v>
       </c>
       <c r="B134" t="n">
-        <v>0.003741234375789463</v>
+        <v>0.00394130320316865</v>
       </c>
     </row>
     <row r="135">
@@ -1514,7 +1514,7 @@
         <v>66.5</v>
       </c>
       <c r="B135" t="n">
-        <v>0.003470920037694201</v>
+        <v>0.00394955714673807</v>
       </c>
     </row>
     <row r="136">
@@ -1522,7 +1522,7 @@
         <v>67</v>
       </c>
       <c r="B136" t="n">
-        <v>0.003890170043762246</v>
+        <v>0.003148019270151784</v>
       </c>
     </row>
     <row r="137">
@@ -1530,7 +1530,7 @@
         <v>67.5</v>
       </c>
       <c r="B137" t="n">
-        <v>0.003948667553134365</v>
+        <v>0.004326888088161056</v>
       </c>
     </row>
     <row r="138">
@@ -1538,7 +1538,7 @@
         <v>68</v>
       </c>
       <c r="B138" t="n">
-        <v>0.00263405949500754</v>
+        <v>0.002751746681439573</v>
       </c>
     </row>
     <row r="139">
@@ -1546,7 +1546,7 @@
         <v>68.5</v>
       </c>
       <c r="B139" t="n">
-        <v>0.003764887922179007</v>
+        <v>0.003404595157208373</v>
       </c>
     </row>
     <row r="140">
@@ -1554,7 +1554,7 @@
         <v>69</v>
       </c>
       <c r="B140" t="n">
-        <v>0.003577701500023494</v>
+        <v>0.003392913542522973</v>
       </c>
     </row>
     <row r="141">
@@ -1562,7 +1562,7 @@
         <v>69.5</v>
       </c>
       <c r="B141" t="n">
-        <v>0.002708941361108218</v>
+        <v>0.003559375507757695</v>
       </c>
     </row>
     <row r="142">
@@ -1570,7 +1570,7 @@
         <v>70</v>
       </c>
       <c r="B142" t="n">
-        <v>0.003633701053848971</v>
+        <v>0.003037950760526262</v>
       </c>
     </row>
     <row r="143">
@@ -1578,7 +1578,7 @@
         <v>70.5</v>
       </c>
       <c r="B143" t="n">
-        <v>0.002633195289043974</v>
+        <v>0.002272739598582164</v>
       </c>
     </row>
     <row r="144">
@@ -1586,7 +1586,7 @@
         <v>71</v>
       </c>
       <c r="B144" t="n">
-        <v>0.002688520376272336</v>
+        <v>0.001950173126420381</v>
       </c>
     </row>
     <row r="145">
@@ -1594,7 +1594,7 @@
         <v>71.5</v>
       </c>
       <c r="B145" t="n">
-        <v>0.001912852656292581</v>
+        <v>0.002248392154481682</v>
       </c>
     </row>
     <row r="146">
@@ -1602,7 +1602,7 @@
         <v>72</v>
       </c>
       <c r="B146" t="n">
-        <v>0.002917774002336314</v>
+        <v>0.002314515219396656</v>
       </c>
     </row>
     <row r="147">
@@ -1610,7 +1610,7 @@
         <v>72.5</v>
       </c>
       <c r="B147" t="n">
-        <v>0.001506287295167262</v>
+        <v>0.001949449259523711</v>
       </c>
     </row>
     <row r="148">
@@ -1618,7 +1618,7 @@
         <v>73</v>
       </c>
       <c r="B148" t="n">
-        <v>0.002671258993938387</v>
+        <v>0.002750160540518979</v>
       </c>
     </row>
     <row r="149">
@@ -1626,7 +1626,7 @@
         <v>73.5</v>
       </c>
       <c r="B149" t="n">
-        <v>0.001293019598437489</v>
+        <v>0.001808356086551173</v>
       </c>
     </row>
     <row r="150">
@@ -1634,7 +1634,7 @@
         <v>74</v>
       </c>
       <c r="B150" t="n">
-        <v>0.001244571167574931</v>
+        <v>0.001383400614695436</v>
       </c>
     </row>
     <row r="151">
@@ -1642,7 +1642,7 @@
         <v>74.5</v>
       </c>
       <c r="B151" t="n">
-        <v>0.002425708083352576</v>
+        <v>0.001634453877079884</v>
       </c>
     </row>
     <row r="152">
@@ -1650,7 +1650,7 @@
         <v>75</v>
       </c>
       <c r="B152" t="n">
-        <v>0.001810450029164599</v>
+        <v>0.002146167448413408</v>
       </c>
     </row>
     <row r="153">
@@ -1658,7 +1658,7 @@
         <v>75.5</v>
       </c>
       <c r="B153" t="n">
-        <v>0.002203754585027527</v>
+        <v>0.001083596921434239</v>
       </c>
     </row>
     <row r="154">
@@ -1666,7 +1666,7 @@
         <v>76</v>
       </c>
       <c r="B154" t="n">
-        <v>0.001346091896336985</v>
+        <v>0.001743203392530024</v>
       </c>
     </row>
     <row r="155">
@@ -1674,7 +1674,7 @@
         <v>76.5</v>
       </c>
       <c r="B155" t="n">
-        <v>0.001520109775935575</v>
+        <v>0.0009735860113407778</v>
       </c>
     </row>
     <row r="156">
@@ -1682,7 +1682,7 @@
         <v>77</v>
       </c>
       <c r="B156" t="n">
-        <v>0.001234657412981938</v>
+        <v>0.002332020822450245</v>
       </c>
     </row>
     <row r="157">
@@ -1690,7 +1690,7 @@
         <v>77.5</v>
       </c>
       <c r="B157" t="n">
-        <v>0.0009078050587664564</v>
+        <v>0.001751913525611423</v>
       </c>
     </row>
     <row r="158">
@@ -1698,7 +1698,7 @@
         <v>78</v>
       </c>
       <c r="B158" t="n">
-        <v>0.001566283193991195</v>
+        <v>0.0006720476293485497</v>
       </c>
     </row>
     <row r="159">
@@ -1706,7 +1706,7 @@
         <v>78.5</v>
       </c>
       <c r="B159" t="n">
-        <v>0.0008550431787406536</v>
+        <v>0.0007890835120441351</v>
       </c>
     </row>
     <row r="160">
@@ -1714,7 +1714,7 @@
         <v>79</v>
       </c>
       <c r="B160" t="n">
-        <v>0.001527872927545207</v>
+        <v>0.0006296577097419841</v>
       </c>
     </row>
     <row r="161">
@@ -1722,7 +1722,7 @@
         <v>79.5</v>
       </c>
       <c r="B161" t="n">
-        <v>0.001494948630323082</v>
+        <v>0.001647281975793457</v>
       </c>
     </row>
     <row r="162">
@@ -1730,7 +1730,7 @@
         <v>80</v>
       </c>
       <c r="B162" t="n">
-        <v>0.001451898590221041</v>
+        <v>0.0003523729664594389</v>
       </c>
     </row>
     <row r="163">
@@ -1738,7 +1738,7 @@
         <v>80.5</v>
       </c>
       <c r="B163" t="n">
-        <v>0.0003896589681008331</v>
+        <v>0.000674763507460609</v>
       </c>
     </row>
     <row r="164">
@@ -1746,7 +1746,7 @@
         <v>81</v>
       </c>
       <c r="B164" t="n">
-        <v>0.001709245364768305</v>
+        <v>0.0006477590525316583</v>
       </c>
     </row>
     <row r="165">
@@ -1754,7 +1754,7 @@
         <v>81.5</v>
       </c>
       <c r="B165" t="n">
-        <v>0.0007365722240506953</v>
+        <v>0.001707025441329627</v>
       </c>
     </row>
     <row r="166">
@@ -1762,7 +1762,7 @@
         <v>82</v>
       </c>
       <c r="B166" t="n">
-        <v>0.001359029847219654</v>
+        <v>0.000922681925468955</v>
       </c>
     </row>
     <row r="167">
@@ -1770,7 +1770,7 @@
         <v>82.5</v>
       </c>
       <c r="B167" t="n">
-        <v>0.00169896110366046</v>
+        <v>8.067043484949043e-05</v>
       </c>
     </row>
     <row r="168">
@@ -1778,7 +1778,7 @@
         <v>83</v>
       </c>
       <c r="B168" t="n">
-        <v>0.0004559636821429346</v>
+        <v>0.00122542695044423</v>
       </c>
     </row>
     <row r="169">
@@ -1786,7 +1786,7 @@
         <v>83.5</v>
       </c>
       <c r="B169" t="n">
-        <v>0.001548417257810438</v>
+        <v>0.0004539497955585936</v>
       </c>
     </row>
     <row r="170">
@@ -1794,7 +1794,7 @@
         <v>84</v>
       </c>
       <c r="B170" t="n">
-        <v>0.001456894549194217</v>
+        <v>0.001363991812255928</v>
       </c>
     </row>
     <row r="171">
@@ -1802,7 +1802,7 @@
         <v>84.5</v>
       </c>
       <c r="B171" t="n">
-        <v>0.001605149520505827</v>
+        <v>-2.675946752881157e-05</v>
       </c>
     </row>
     <row r="172">
@@ -1810,7 +1810,7 @@
         <v>85</v>
       </c>
       <c r="B172" t="n">
-        <v>0.00119847628836227</v>
+        <v>0.0004977727933350103</v>
       </c>
     </row>
     <row r="173">
@@ -1818,7 +1818,7 @@
         <v>85.5</v>
       </c>
       <c r="B173" t="n">
-        <v>0.001195034894900204</v>
+        <v>0.0013905597478442</v>
       </c>
     </row>
     <row r="174">
@@ -1826,7 +1826,7 @@
         <v>86</v>
       </c>
       <c r="B174" t="n">
-        <v>0.0004804081459320922</v>
+        <v>0.0007463914911776842</v>
       </c>
     </row>
     <row r="175">
@@ -1834,7 +1834,7 @@
         <v>86.5</v>
       </c>
       <c r="B175" t="n">
-        <v>0.001450838907093669</v>
+        <v>0.0009833977379629128</v>
       </c>
     </row>
     <row r="176">
@@ -1842,7 +1842,7 @@
         <v>87</v>
       </c>
       <c r="B176" t="n">
-        <v>0.001272316182376962</v>
+        <v>0.0003866900923888943</v>
       </c>
     </row>
     <row r="177">
@@ -1850,7 +1850,7 @@
         <v>87.5</v>
       </c>
       <c r="B177" t="n">
-        <v>8.475485404826769e-07</v>
+        <v>3.481018001275701e-05</v>
       </c>
     </row>
     <row r="178">
@@ -1858,7 +1858,7 @@
         <v>88</v>
       </c>
       <c r="B178" t="n">
-        <v>0.0003070066650076022</v>
+        <v>4.010357723483566e-05</v>
       </c>
     </row>
     <row r="179">
@@ -1866,7 +1866,7 @@
         <v>88.5</v>
       </c>
       <c r="B179" t="n">
-        <v>0.001168192300809761</v>
+        <v>0.001359256310199126</v>
       </c>
     </row>
     <row r="180">
@@ -1874,7 +1874,7 @@
         <v>89</v>
       </c>
       <c r="B180" t="n">
-        <v>0.0009324510013430857</v>
+        <v>0.0003712342662384601</v>
       </c>
     </row>
     <row r="181">
@@ -1882,7 +1882,7 @@
         <v>89.5</v>
       </c>
       <c r="B181" t="n">
-        <v>0.0003511834450521714</v>
+        <v>-0.0001813357783101818</v>
       </c>
     </row>
     <row r="182">
@@ -1890,7 +1890,7 @@
         <v>90</v>
       </c>
       <c r="B182" t="n">
-        <v>0.001094372570919677</v>
+        <v>-0.0001739161463682427</v>
       </c>
     </row>
     <row r="183">
@@ -1898,7 +1898,7 @@
         <v>90.5</v>
       </c>
       <c r="B183" t="n">
-        <v>6.930200542692663e-05</v>
+        <v>0.001332354781073538</v>
       </c>
     </row>
     <row r="184">
@@ -1906,7 +1906,7 @@
         <v>91</v>
       </c>
       <c r="B184" t="n">
-        <v>0.0008081769500868307</v>
+        <v>0.0003199670968198365</v>
       </c>
     </row>
     <row r="185">
@@ -1914,7 +1914,7 @@
         <v>91.5</v>
       </c>
       <c r="B185" t="n">
-        <v>0.0002429060651396497</v>
+        <v>0.0006826755196882341</v>
       </c>
     </row>
     <row r="186">
@@ -1922,7 +1922,7 @@
         <v>92</v>
       </c>
       <c r="B186" t="n">
-        <v>-4.014502188817086e-05</v>
+        <v>0.0001571859046859152</v>
       </c>
     </row>
     <row r="187">
@@ -1930,7 +1930,7 @@
         <v>92.5</v>
       </c>
       <c r="B187" t="n">
-        <v>0.001256842950014352</v>
+        <v>-0.0002021158843819361</v>
       </c>
     </row>
     <row r="188">
@@ -1938,7 +1938,7 @@
         <v>93</v>
       </c>
       <c r="B188" t="n">
-        <v>0.0002530939991056264</v>
+        <v>0.001232108510518704</v>
       </c>
     </row>
     <row r="189">
@@ -1946,7 +1946,7 @@
         <v>93.5</v>
       </c>
       <c r="B189" t="n">
-        <v>-0.0004863752399315306</v>
+        <v>-0.0001657739469562112</v>
       </c>
     </row>
     <row r="190">
@@ -1954,7 +1954,7 @@
         <v>94</v>
       </c>
       <c r="B190" t="n">
-        <v>0.0004289451580591133</v>
+        <v>0.0006215881778006597</v>
       </c>
     </row>
     <row r="191">
@@ -1962,7 +1962,7 @@
         <v>94.5</v>
       </c>
       <c r="B191" t="n">
-        <v>0.0003274008022977163</v>
+        <v>0.000421357261297749</v>
       </c>
     </row>
     <row r="192">
@@ -1970,7 +1970,7 @@
         <v>95</v>
       </c>
       <c r="B192" t="n">
-        <v>0.0002756699605967059</v>
+        <v>0.00115993237567708</v>
       </c>
     </row>
     <row r="193">
@@ -1978,7 +1978,7 @@
         <v>95.5</v>
       </c>
       <c r="B193" t="n">
-        <v>0.0004389555966143989</v>
+        <v>0.0001522410795986551</v>
       </c>
     </row>
     <row r="194">
@@ -1986,7 +1986,7 @@
         <v>96</v>
       </c>
       <c r="B194" t="n">
-        <v>0.0002215877486111418</v>
+        <v>0.001146105291822838</v>
       </c>
     </row>
     <row r="195">
@@ -1994,7 +1994,7 @@
         <v>96.5</v>
       </c>
       <c r="B195" t="n">
-        <v>-9.46664511559252e-05</v>
+        <v>6.941399232083048e-07</v>
       </c>
     </row>
     <row r="196">
@@ -2002,7 +2002,7 @@
         <v>97</v>
       </c>
       <c r="B196" t="n">
-        <v>-0.0004676752472458347</v>
+        <v>0.001028395087510863</v>
       </c>
     </row>
     <row r="197">
@@ -2010,7 +2010,7 @@
         <v>97.5</v>
       </c>
       <c r="B197" t="n">
-        <v>0.0008086102169332235</v>
+        <v>-0.0002617170078759976</v>
       </c>
     </row>
     <row r="198">
@@ -2018,7 +2018,7 @@
         <v>98</v>
       </c>
       <c r="B198" t="n">
-        <v>0.000732425542253835</v>
+        <v>-0.0001270557749021156</v>
       </c>
     </row>
     <row r="199">
@@ -2026,7 +2026,7 @@
         <v>98.5</v>
       </c>
       <c r="B199" t="n">
-        <v>0.0005992633873231526</v>
+        <v>2.222290002529975e-05</v>
       </c>
     </row>
     <row r="200">
@@ -2034,7 +2034,7 @@
         <v>99</v>
       </c>
       <c r="B200" t="n">
-        <v>-0.0002762687896175901</v>
+        <v>-2.481938696675371e-05</v>
       </c>
     </row>
     <row r="201">
@@ -2042,7 +2042,7 @@
         <v>99.5</v>
       </c>
       <c r="B201" t="n">
-        <v>1.541152640638943e-05</v>
+        <v>8.797894159852521e-05</v>
       </c>
     </row>
     <row r="202">
@@ -2050,7 +2050,7 @@
         <v>100</v>
       </c>
       <c r="B202" t="n">
-        <v>0.0003478945999507092</v>
+        <v>0.0001515957028367253</v>
       </c>
     </row>
     <row r="203">
@@ -2058,7 +2058,7 @@
         <v>100.5</v>
       </c>
       <c r="B203" t="n">
-        <v>0.0001282474445738092</v>
+        <v>0.0004469980253689731</v>
       </c>
     </row>
     <row r="204">
@@ -2066,7 +2066,7 @@
         <v>101</v>
       </c>
       <c r="B204" t="n">
-        <v>9.269482235327913e-05</v>
+        <v>0.0003111791244508227</v>
       </c>
     </row>
     <row r="205">
@@ -2074,7 +2074,7 @@
         <v>101.5</v>
       </c>
       <c r="B205" t="n">
-        <v>0.0006941723554898798</v>
+        <v>0.0005478981741706071</v>
       </c>
     </row>
     <row r="206">
@@ -2082,7 +2082,7 @@
         <v>102</v>
       </c>
       <c r="B206" t="n">
-        <v>0.0002794640199476198</v>
+        <v>-0.000521665566045313</v>
       </c>
     </row>
     <row r="207">
@@ -2090,7 +2090,7 @@
         <v>102.5</v>
       </c>
       <c r="B207" t="n">
-        <v>-0.0001667870725040954</v>
+        <v>0.000942114633224542</v>
       </c>
     </row>
     <row r="208">
@@ -2098,7 +2098,7 @@
         <v>103</v>
       </c>
       <c r="B208" t="n">
-        <v>-8.595064792048422e-05</v>
+        <v>-0.000446100725637116</v>
       </c>
     </row>
     <row r="209">
@@ -2106,7 +2106,7 @@
         <v>103.5</v>
       </c>
       <c r="B209" t="n">
-        <v>-0.0002819014169790066</v>
+        <v>0.000888918295538862</v>
       </c>
     </row>
     <row r="210">
@@ -2114,7 +2114,7 @@
         <v>104</v>
       </c>
       <c r="B210" t="n">
-        <v>0.0008752152508992748</v>
+        <v>0.0004284118644983707</v>
       </c>
     </row>
     <row r="211">
@@ -2122,7 +2122,7 @@
         <v>104.5</v>
       </c>
       <c r="B211" t="n">
-        <v>0.0002123500651604518</v>
+        <v>0.0003491625472013894</v>
       </c>
     </row>
     <row r="212">
@@ -2130,7 +2130,7 @@
         <v>105</v>
       </c>
       <c r="B212" t="n">
-        <v>0.0008647596420892466</v>
+        <v>-0.0005984312821481801</v>
       </c>
     </row>
     <row r="213">
@@ -2138,7 +2138,7 @@
         <v>105.5</v>
       </c>
       <c r="B213" t="n">
-        <v>0.0006150718438545072</v>
+        <v>0.0001619204925310802</v>
       </c>
     </row>
     <row r="214">
@@ -2146,7 +2146,7 @@
         <v>106</v>
       </c>
       <c r="B214" t="n">
-        <v>0.0001765290066032292</v>
+        <v>0.0009300497289452161</v>
       </c>
     </row>
     <row r="215">
@@ -2154,7 +2154,7 @@
         <v>106.5</v>
       </c>
       <c r="B215" t="n">
-        <v>-0.0006842745296843645</v>
+        <v>0.0004424225082227402</v>
       </c>
     </row>
     <row r="216">
@@ -2162,7 +2162,7 @@
         <v>107</v>
       </c>
       <c r="B216" t="n">
-        <v>-0.0004189618322770767</v>
+        <v>-0.000725928452829842</v>
       </c>
     </row>
     <row r="217">
@@ -2170,7 +2170,7 @@
         <v>107.5</v>
       </c>
       <c r="B217" t="n">
-        <v>0.0006410786076278</v>
+        <v>-0.0002078629772562752</v>
       </c>
     </row>
     <row r="218">
@@ -2178,7 +2178,7 @@
         <v>108</v>
       </c>
       <c r="B218" t="n">
-        <v>0.0004791112919569991</v>
+        <v>-0.0003138598594091238</v>
       </c>
     </row>
     <row r="219">
@@ -2186,7 +2186,7 @@
         <v>108.5</v>
       </c>
       <c r="B219" t="n">
-        <v>0.0008955103242114109</v>
+        <v>-0.0003611347548148961</v>
       </c>
     </row>
     <row r="220">
@@ -2194,7 +2194,7 @@
         <v>109</v>
       </c>
       <c r="B220" t="n">
-        <v>0.0008532912144233566</v>
+        <v>-0.0002335750926963523</v>
       </c>
     </row>
     <row r="221">
@@ -2202,7 +2202,7 @@
         <v>109.5</v>
       </c>
       <c r="B221" t="n">
-        <v>-0.0004281041800644329</v>
+        <v>-0.0002132902901671678</v>
       </c>
     </row>
     <row r="222">
@@ -2210,7 +2210,7 @@
         <v>110</v>
       </c>
       <c r="B222" t="n">
-        <v>3.666809784402115e-05</v>
+        <v>-0.0006091192626593973</v>
       </c>
     </row>
     <row r="223">
@@ -2218,7 +2218,7 @@
         <v>110.5</v>
       </c>
       <c r="B223" t="n">
-        <v>-0.0004609740774991709</v>
+        <v>-0.0002749254976222231</v>
       </c>
     </row>
     <row r="224">
@@ -2226,7 +2226,7 @@
         <v>111</v>
       </c>
       <c r="B224" t="n">
-        <v>0.0002486021107952495</v>
+        <v>-8.159566085828341e-05</v>
       </c>
     </row>
     <row r="225">
@@ -2234,7 +2234,7 @@
         <v>111.5</v>
       </c>
       <c r="B225" t="n">
-        <v>0.0004982533733549894</v>
+        <v>-0.0002571775213851339</v>
       </c>
     </row>
     <row r="226">
@@ -2242,7 +2242,7 @@
         <v>112</v>
       </c>
       <c r="B226" t="n">
-        <v>-0.0005981304556441933</v>
+        <v>-0.0004991818270458177</v>
       </c>
     </row>
     <row r="227">
@@ -2250,7 +2250,7 @@
         <v>112.5</v>
       </c>
       <c r="B227" t="n">
-        <v>0.0001988233064757487</v>
+        <v>0.0007240802436580811</v>
       </c>
     </row>
     <row r="228">
@@ -2258,7 +2258,7 @@
         <v>113</v>
       </c>
       <c r="B228" t="n">
-        <v>-0.0006288545606993425</v>
+        <v>-6.778517681585688e-05</v>
       </c>
     </row>
     <row r="229">
@@ -2266,7 +2266,7 @@
         <v>113.5</v>
       </c>
       <c r="B229" t="n">
-        <v>0.0006643905150505983</v>
+        <v>-0.0006347403239415383</v>
       </c>
     </row>
     <row r="230">
@@ -2274,7 +2274,7 @@
         <v>114</v>
       </c>
       <c r="B230" t="n">
-        <v>0.0005423832364135315</v>
+        <v>-0.0003760908376326526</v>
       </c>
     </row>
     <row r="231">
@@ -2282,7 +2282,7 @@
         <v>114.5</v>
       </c>
       <c r="B231" t="n">
-        <v>-0.0006493075544115211</v>
+        <v>0.0004167259203448117</v>
       </c>
     </row>
     <row r="232">
@@ -2290,7 +2290,7 @@
         <v>115</v>
       </c>
       <c r="B232" t="n">
-        <v>0.0007056660007371223</v>
+        <v>0.0002649053269883049</v>
       </c>
     </row>
     <row r="233">
@@ -2298,7 +2298,7 @@
         <v>115.5</v>
       </c>
       <c r="B233" t="n">
-        <v>0.000195252169518786</v>
+        <v>5.236404881439928e-05</v>
       </c>
     </row>
     <row r="234">
@@ -2306,7 +2306,7 @@
         <v>116</v>
       </c>
       <c r="B234" t="n">
-        <v>-4.905068707092991e-05</v>
+        <v>-3.049881922437977e-05</v>
       </c>
     </row>
     <row r="235">
@@ -2314,7 +2314,7 @@
         <v>116.5</v>
       </c>
       <c r="B235" t="n">
-        <v>0.0007379140540948255</v>
+        <v>-0.0007188718931660623</v>
       </c>
     </row>
     <row r="236">
@@ -2322,7 +2322,7 @@
         <v>117</v>
       </c>
       <c r="B236" t="n">
-        <v>0.0008164102821809732</v>
+        <v>0.000753015676688</v>
       </c>
     </row>
     <row r="237">
@@ -2330,7 +2330,7 @@
         <v>117.5</v>
       </c>
       <c r="B237" t="n">
-        <v>-0.0008255492502432418</v>
+        <v>-0.0002897556604095942</v>
       </c>
     </row>
     <row r="238">
@@ -2338,7 +2338,7 @@
         <v>118</v>
       </c>
       <c r="B238" t="n">
-        <v>0.0001820195828602581</v>
+        <v>6.53370212901438e-05</v>
       </c>
     </row>
     <row r="239">
@@ -2346,7 +2346,7 @@
         <v>118.5</v>
       </c>
       <c r="B239" t="n">
-        <v>-0.000823577415937014</v>
+        <v>-3.321289584629448e-05</v>
       </c>
     </row>
     <row r="240">
@@ -2354,7 +2354,7 @@
         <v>119</v>
       </c>
       <c r="B240" t="n">
-        <v>0.0005621538629945476</v>
+        <v>-0.0003414751556752171</v>
       </c>
     </row>
     <row r="241">
@@ -2362,7 +2362,7 @@
         <v>119.5</v>
       </c>
       <c r="B241" t="n">
-        <v>-0.0002385720554310718</v>
+        <v>0.0003540132353851246</v>
       </c>
     </row>
     <row r="242">
@@ -2370,7 +2370,7 @@
         <v>120</v>
       </c>
       <c r="B242" t="n">
-        <v>-0.0004717490216214593</v>
+        <v>-0.0006134942369195353</v>
       </c>
     </row>
     <row r="243">
@@ -2378,7 +2378,7 @@
         <v>120.5</v>
       </c>
       <c r="B243" t="n">
-        <v>-0.0005474324543397447</v>
+        <v>0.0002989892300429766</v>
       </c>
     </row>
     <row r="244">
@@ -2386,7 +2386,7 @@
         <v>121</v>
       </c>
       <c r="B244" t="n">
-        <v>-0.0004393886198205769</v>
+        <v>0.0004715881868480375</v>
       </c>
     </row>
     <row r="245">
@@ -2394,7 +2394,7 @@
         <v>121.5</v>
       </c>
       <c r="B245" t="n">
-        <v>0.0003560492606003253</v>
+        <v>0.0004475327044058102</v>
       </c>
     </row>
     <row r="246">
@@ -2402,7 +2402,7 @@
         <v>122</v>
       </c>
       <c r="B246" t="n">
-        <v>0.0001038648892242702</v>
+        <v>-0.0001478723339042238</v>
       </c>
     </row>
     <row r="247">
@@ -2410,7 +2410,7 @@
         <v>122.5</v>
       </c>
       <c r="B247" t="n">
-        <v>-0.0007094341554981119</v>
+        <v>0.0002471896307054835</v>
       </c>
     </row>
     <row r="248">
@@ -2418,7 +2418,7 @@
         <v>123</v>
       </c>
       <c r="B248" t="n">
-        <v>0.0001053285328639921</v>
+        <v>0.0006367063658077978</v>
       </c>
     </row>
     <row r="249">
@@ -2426,7 +2426,7 @@
         <v>123.5</v>
       </c>
       <c r="B249" t="n">
-        <v>0.0003447935396696882</v>
+        <v>7.648716478281069e-05</v>
       </c>
     </row>
     <row r="250">
@@ -2434,7 +2434,7 @@
         <v>124</v>
       </c>
       <c r="B250" t="n">
-        <v>0.0005361869115969478</v>
+        <v>0.0006006390737715759</v>
       </c>
     </row>
     <row r="251">
@@ -2442,7 +2442,7 @@
         <v>124.5</v>
       </c>
       <c r="B251" t="n">
-        <v>0.0002954562592470581</v>
+        <v>0.0003964710861509017</v>
       </c>
     </row>
     <row r="252">
@@ -2450,7 +2450,7 @@
         <v>125</v>
       </c>
       <c r="B252" t="n">
-        <v>-0.0005632264931592803</v>
+        <v>-0.0007765003752796203</v>
       </c>
     </row>
     <row r="253">
@@ -2458,7 +2458,7 @@
         <v>125.5</v>
       </c>
       <c r="B253" t="n">
-        <v>0.0003688208688270314</v>
+        <v>0.000619654084398173</v>
       </c>
     </row>
     <row r="254">
@@ -2466,7 +2466,7 @@
         <v>126</v>
       </c>
       <c r="B254" t="n">
-        <v>-0.0006500834751565453</v>
+        <v>0.0001144472187844398</v>
       </c>
     </row>
     <row r="255">
@@ -2474,7 +2474,7 @@
         <v>126.5</v>
       </c>
       <c r="B255" t="n">
-        <v>0.0003043288657275969</v>
+        <v>-0.0008343047443018638</v>
       </c>
     </row>
     <row r="256">
@@ -2482,7 +2482,7 @@
         <v>127</v>
       </c>
       <c r="B256" t="n">
-        <v>0.0005137197635098386</v>
+        <v>-0.0003095409097759871</v>
       </c>
     </row>
     <row r="257">
@@ -2490,7 +2490,7 @@
         <v>127.5</v>
       </c>
       <c r="B257" t="n">
-        <v>-0.0007152167602212797</v>
+        <v>0.0004556828133945955</v>
       </c>
     </row>
     <row r="258">
@@ -2498,7 +2498,7 @@
         <v>128</v>
       </c>
       <c r="B258" t="n">
-        <v>-0.000719077246157721</v>
+        <v>0.0003884809840456896</v>
       </c>
     </row>
     <row r="259">
@@ -2506,7 +2506,7 @@
         <v>128.5</v>
       </c>
       <c r="B259" t="n">
-        <v>0.0006316841780598259</v>
+        <v>-0.0003267115127999158</v>
       </c>
     </row>
     <row r="260">
@@ -2514,7 +2514,7 @@
         <v>129</v>
       </c>
       <c r="B260" t="n">
-        <v>1.746220794999355e-05</v>
+        <v>0.0007526735879504373</v>
       </c>
     </row>
     <row r="261">
@@ -2522,7 +2522,7 @@
         <v>129.5</v>
       </c>
       <c r="B261" t="n">
-        <v>-0.0006805065808716888</v>
+        <v>-0.000852607360046473</v>
       </c>
     </row>
     <row r="262">
@@ -2530,7 +2530,7 @@
         <v>130</v>
       </c>
       <c r="B262" t="n">
-        <v>-0.0005078496686070492</v>
+        <v>0.0003391318516452735</v>
       </c>
     </row>
     <row r="263">
@@ -2538,7 +2538,7 @@
         <v>130.5</v>
       </c>
       <c r="B263" t="n">
-        <v>-0.0004378103320207988</v>
+        <v>-0.0001857756488444619</v>
       </c>
     </row>
     <row r="264">
@@ -2546,7 +2546,7 @@
         <v>131</v>
       </c>
       <c r="B264" t="n">
-        <v>-0.0002600645260623266</v>
+        <v>-0.000225687509448968</v>
       </c>
     </row>
     <row r="265">
@@ -2554,7 +2554,7 @@
         <v>131.5</v>
       </c>
       <c r="B265" t="n">
-        <v>-0.0004531487690209131</v>
+        <v>0.0004425715613976573</v>
       </c>
     </row>
     <row r="266">
@@ -2562,7 +2562,7 @@
         <v>132</v>
       </c>
       <c r="B266" t="n">
-        <v>-0.0003543085808464868</v>
+        <v>0.0001890398775217608</v>
       </c>
     </row>
     <row r="267">
@@ -2570,7 +2570,7 @@
         <v>132.5</v>
       </c>
       <c r="B267" t="n">
-        <v>-0.000122145645655227</v>
+        <v>-0.000805433155791743</v>
       </c>
     </row>
     <row r="268">
@@ -2578,7 +2578,7 @@
         <v>133</v>
       </c>
       <c r="B268" t="n">
-        <v>-7.89294652488714e-05</v>
+        <v>-5.418522964241204e-05</v>
       </c>
     </row>
     <row r="269">
@@ -2586,7 +2586,7 @@
         <v>133.5</v>
       </c>
       <c r="B269" t="n">
-        <v>-0.0005686717161147195</v>
+        <v>0.000555330861891054</v>
       </c>
     </row>
     <row r="270">
@@ -2594,7 +2594,7 @@
         <v>134</v>
       </c>
       <c r="B270" t="n">
-        <v>0.0001051829470653633</v>
+        <v>-0.0006124656120275219</v>
       </c>
     </row>
     <row r="271">
@@ -2602,7 +2602,7 @@
         <v>134.5</v>
       </c>
       <c r="B271" t="n">
-        <v>-0.0004117394857696117</v>
+        <v>0.0007399316146500462</v>
       </c>
     </row>
     <row r="272">
@@ -2610,7 +2610,7 @@
         <v>135</v>
       </c>
       <c r="B272" t="n">
-        <v>0.0008585619299363692</v>
+        <v>0.0007677007441358953</v>
       </c>
     </row>
     <row r="273">
@@ -2618,7 +2618,7 @@
         <v>135.5</v>
       </c>
       <c r="B273" t="n">
-        <v>-8.15397122605203e-05</v>
+        <v>-0.000486891500251015</v>
       </c>
     </row>
     <row r="274">
@@ -2626,7 +2626,7 @@
         <v>136</v>
       </c>
       <c r="B274" t="n">
-        <v>-0.0003610950447093045</v>
+        <v>0.0006943462982950001</v>
       </c>
     </row>
     <row r="275">
@@ -2634,7 +2634,7 @@
         <v>136.5</v>
       </c>
       <c r="B275" t="n">
-        <v>0.0003561966528193956</v>
+        <v>0.0006400064642556953</v>
       </c>
     </row>
     <row r="276">
@@ -2642,7 +2642,7 @@
         <v>137</v>
       </c>
       <c r="B276" t="n">
-        <v>0.0002808182260076849</v>
+        <v>-0.0003799557011051507</v>
       </c>
     </row>
     <row r="277">
@@ -2650,7 +2650,7 @@
         <v>137.5</v>
       </c>
       <c r="B277" t="n">
-        <v>-0.0004029385898195311</v>
+        <v>0.0004972452844719984</v>
       </c>
     </row>
     <row r="278">
@@ -2658,7 +2658,7 @@
         <v>138</v>
       </c>
       <c r="B278" t="n">
-        <v>0.0003019968037482112</v>
+        <v>0.0005820831259371326</v>
       </c>
     </row>
     <row r="279">
@@ -2666,7 +2666,7 @@
         <v>138.5</v>
       </c>
       <c r="B279" t="n">
-        <v>-0.0006173921736894374</v>
+        <v>0.0002259032076805995</v>
       </c>
     </row>
     <row r="280">
@@ -2674,7 +2674,7 @@
         <v>139</v>
       </c>
       <c r="B280" t="n">
-        <v>0.0007483479271428547</v>
+        <v>0.000147441482906596</v>
       </c>
     </row>
     <row r="281">
@@ -2682,7 +2682,7 @@
         <v>139.5</v>
       </c>
       <c r="B281" t="n">
-        <v>-0.0005630699495128773</v>
+        <v>-0.0001851544394653296</v>
       </c>
     </row>
     <row r="282">
@@ -2690,7 +2690,7 @@
         <v>140</v>
       </c>
       <c r="B282" t="n">
-        <v>-0.0005097660070174609</v>
+        <v>3.10600985358225e-05</v>
       </c>
     </row>
     <row r="283">
@@ -2698,7 +2698,7 @@
         <v>140.5</v>
       </c>
       <c r="B283" t="n">
-        <v>-0.0001510975193363417</v>
+        <v>-0.0006656585247341582</v>
       </c>
     </row>
     <row r="284">
@@ -2706,7 +2706,7 @@
         <v>141</v>
       </c>
       <c r="B284" t="n">
-        <v>0.0005292170670779061</v>
+        <v>0.0008609210444968609</v>
       </c>
     </row>
     <row r="285">
@@ -2714,7 +2714,7 @@
         <v>141.5</v>
       </c>
       <c r="B285" t="n">
-        <v>-0.0003552961576681136</v>
+        <v>-0.0004077960927431726</v>
       </c>
     </row>
     <row r="286">
@@ -2722,7 +2722,7 @@
         <v>142</v>
       </c>
       <c r="B286" t="n">
-        <v>0.0003105776178339496</v>
+        <v>8.11564747970912e-05</v>
       </c>
     </row>
     <row r="287">
@@ -2730,7 +2730,7 @@
         <v>142.5</v>
       </c>
       <c r="B287" t="n">
-        <v>-6.756410172023641e-05</v>
+        <v>-0.0002022594533319939</v>
       </c>
     </row>
     <row r="288">
@@ -2738,7 +2738,7 @@
         <v>143</v>
       </c>
       <c r="B288" t="n">
-        <v>0.0006483572016903746</v>
+        <v>0.0007193372281363712</v>
       </c>
     </row>
     <row r="289">
@@ -2746,7 +2746,7 @@
         <v>143.5</v>
       </c>
       <c r="B289" t="n">
-        <v>-0.000472040300665692</v>
+        <v>-0.0001627395904898109</v>
       </c>
     </row>
     <row r="290">
@@ -2754,7 +2754,7 @@
         <v>144</v>
       </c>
       <c r="B290" t="n">
-        <v>0.0006914624817616154</v>
+        <v>-2.467371497284459e-05</v>
       </c>
     </row>
     <row r="291">
@@ -2762,7 +2762,7 @@
         <v>144.5</v>
       </c>
       <c r="B291" t="n">
-        <v>0.000749962307517454</v>
+        <v>-0.0003206883147186908</v>
       </c>
     </row>
     <row r="292">
@@ -2770,7 +2770,7 @@
         <v>145</v>
       </c>
       <c r="B292" t="n">
-        <v>8.575813717328864e-05</v>
+        <v>0.0007726930811214031</v>
       </c>
     </row>
     <row r="293">
@@ -2778,7 +2778,7 @@
         <v>145.5</v>
       </c>
       <c r="B293" t="n">
-        <v>-0.0001292703948501435</v>
+        <v>-0.0007004611778279915</v>
       </c>
     </row>
     <row r="294">
@@ -2786,7 +2786,7 @@
         <v>146</v>
       </c>
       <c r="B294" t="n">
-        <v>-0.0008662638305994526</v>
+        <v>0.0004992199808059506</v>
       </c>
     </row>
     <row r="295">
@@ -2794,7 +2794,7 @@
         <v>146.5</v>
       </c>
       <c r="B295" t="n">
-        <v>-4.36236455695903e-05</v>
+        <v>0.000849953247854321</v>
       </c>
     </row>
     <row r="296">
@@ -2802,7 +2802,7 @@
         <v>147</v>
       </c>
       <c r="B296" t="n">
-        <v>0.0005772230320462457</v>
+        <v>-0.0005478765058682761</v>
       </c>
     </row>
     <row r="297">
@@ -2810,7 +2810,7 @@
         <v>147.5</v>
       </c>
       <c r="B297" t="n">
-        <v>0.0007852085963361525</v>
+        <v>-0.0003605725713440569</v>
       </c>
     </row>
     <row r="298">
@@ -2818,7 +2818,7 @@
         <v>148</v>
       </c>
       <c r="B298" t="n">
-        <v>-0.0003571709849925256</v>
+        <v>0.0005695900323410877</v>
       </c>
     </row>
     <row r="299">
@@ -2826,7 +2826,7 @@
         <v>148.5</v>
       </c>
       <c r="B299" t="n">
-        <v>0.0005118302281868761</v>
+        <v>-0.000747979874164073</v>
       </c>
     </row>
     <row r="300">
@@ -2834,7 +2834,7 @@
         <v>149</v>
       </c>
       <c r="B300" t="n">
-        <v>-0.000743163394086223</v>
+        <v>0.0004680007968874587</v>
       </c>
     </row>
     <row r="301">
@@ -2842,7 +2842,7 @@
         <v>149.5</v>
       </c>
       <c r="B301" t="n">
-        <v>-3.877693702230665e-05</v>
+        <v>0.0001856810162532007</v>
       </c>
     </row>
     <row r="302">
@@ -2850,7 +2850,7 @@
         <v>150</v>
       </c>
       <c r="B302" t="n">
-        <v>-1.822824668047e-05</v>
+        <v>0.0004886832167159066</v>
       </c>
     </row>
     <row r="303">
@@ -2858,7 +2858,7 @@
         <v>150.5</v>
       </c>
       <c r="B303" t="n">
-        <v>0.0005836055245980673</v>
+        <v>-0.0006280902712865261</v>
       </c>
     </row>
     <row r="304">
@@ -2866,7 +2866,7 @@
         <v>151</v>
       </c>
       <c r="B304" t="n">
-        <v>-0.0008076348719335361</v>
+        <v>-0.0003966659555971942</v>
       </c>
     </row>
     <row r="305">
@@ -2874,7 +2874,7 @@
         <v>151.5</v>
       </c>
       <c r="B305" t="n">
-        <v>-0.0004701344320442396</v>
+        <v>-0.0007158638999877993</v>
       </c>
     </row>
     <row r="306">
@@ -2882,7 +2882,7 @@
         <v>152</v>
       </c>
       <c r="B306" t="n">
-        <v>-0.0002879659398979927</v>
+        <v>0.0007210645529055348</v>
       </c>
     </row>
     <row r="307">
@@ -2890,7 +2890,7 @@
         <v>152.5</v>
       </c>
       <c r="B307" t="n">
-        <v>0.0004538644879178562</v>
+        <v>-0.0005921028538121859</v>
       </c>
     </row>
     <row r="308">
@@ -2898,7 +2898,7 @@
         <v>153</v>
       </c>
       <c r="B308" t="n">
-        <v>0.0007900507371935032</v>
+        <v>-0.0003879946883958868</v>
       </c>
     </row>
     <row r="309">
@@ -2906,7 +2906,7 @@
         <v>153.5</v>
       </c>
       <c r="B309" t="n">
-        <v>0.0005008749741593657</v>
+        <v>3.319797554761766e-05</v>
       </c>
     </row>
     <row r="310">
@@ -2914,7 +2914,7 @@
         <v>154</v>
       </c>
       <c r="B310" t="n">
-        <v>0.0004091434648698359</v>
+        <v>0.0002609876137361368</v>
       </c>
     </row>
     <row r="311">
@@ -2922,7 +2922,7 @@
         <v>154.5</v>
       </c>
       <c r="B311" t="n">
-        <v>-0.0005283804006493505</v>
+        <v>-0.0003641262366503515</v>
       </c>
     </row>
     <row r="312">
@@ -2930,7 +2930,7 @@
         <v>155</v>
       </c>
       <c r="B312" t="n">
-        <v>0.0006112301321201487</v>
+        <v>3.46926797328469e-06</v>
       </c>
     </row>
     <row r="313">
@@ -2938,7 +2938,7 @@
         <v>155.5</v>
       </c>
       <c r="B313" t="n">
-        <v>-0.0005982669454510789</v>
+        <v>0.0002846008806613123</v>
       </c>
     </row>
     <row r="314">
@@ -2946,7 +2946,7 @@
         <v>156</v>
       </c>
       <c r="B314" t="n">
-        <v>-0.0005091048114961429</v>
+        <v>0.0005512387443680977</v>
       </c>
     </row>
     <row r="315">
@@ -2954,7 +2954,7 @@
         <v>156.5</v>
       </c>
       <c r="B315" t="n">
-        <v>-0.0006977033634047671</v>
+        <v>0.0008086654454444813</v>
       </c>
     </row>
     <row r="316">
@@ -2962,7 +2962,7 @@
         <v>157</v>
       </c>
       <c r="B316" t="n">
-        <v>-3.677176502069191e-05</v>
+        <v>-4.568281617107033e-05</v>
       </c>
     </row>
     <row r="317">
@@ -2970,7 +2970,7 @@
         <v>157.5</v>
       </c>
       <c r="B317" t="n">
-        <v>-0.0005186568999923724</v>
+        <v>0.0006937684410512421</v>
       </c>
     </row>
     <row r="318">
@@ -2978,7 +2978,7 @@
         <v>158</v>
       </c>
       <c r="B318" t="n">
-        <v>-2.31198408764863e-05</v>
+        <v>0.0004230896761897683</v>
       </c>
     </row>
     <row r="319">
@@ -2986,7 +2986,7 @@
         <v>158.5</v>
       </c>
       <c r="B319" t="n">
-        <v>0.000368573232255791</v>
+        <v>0.0006206340489281618</v>
       </c>
     </row>
     <row r="320">
@@ -2994,7 +2994,7 @@
         <v>159</v>
       </c>
       <c r="B320" t="n">
-        <v>-0.0005403285909097483</v>
+        <v>0.0008378064273994315</v>
       </c>
     </row>
     <row r="321">
@@ -3002,7 +3002,7 @@
         <v>159.5</v>
       </c>
       <c r="B321" t="n">
-        <v>0.0003531742298213803</v>
+        <v>-9.73316115680349e-05</v>
       </c>
     </row>
     <row r="322">
@@ -3010,7 +3010,7 @@
         <v>160</v>
       </c>
       <c r="B322" t="n">
-        <v>0.0007337128955273083</v>
+        <v>0.0003532981163893362</v>
       </c>
     </row>
     <row r="323">
@@ -3018,7 +3018,7 @@
         <v>160.5</v>
       </c>
       <c r="B323" t="n">
-        <v>0.0005188884412114996</v>
+        <v>-8.885020121445312e-05</v>
       </c>
     </row>
     <row r="324">
@@ -3026,7 +3026,7 @@
         <v>161</v>
       </c>
       <c r="B324" t="n">
-        <v>8.139912445084036e-05</v>
+        <v>0.0006359436679570365</v>
       </c>
     </row>
     <row r="325">
@@ -3034,7 +3034,7 @@
         <v>161.5</v>
       </c>
       <c r="B325" t="n">
-        <v>0.0004683573058778349</v>
+        <v>-0.000215960753380863</v>
       </c>
     </row>
     <row r="326">
@@ -3042,7 +3042,7 @@
         <v>162</v>
       </c>
       <c r="B326" t="n">
-        <v>-0.0002894548539066155</v>
+        <v>-0.000443708407327766</v>
       </c>
     </row>
     <row r="327">
@@ -3050,7 +3050,7 @@
         <v>162.5</v>
       </c>
       <c r="B327" t="n">
-        <v>0.000492507601176018</v>
+        <v>0.0004709944560748135</v>
       </c>
     </row>
     <row r="328">
@@ -3058,7 +3058,7 @@
         <v>163</v>
       </c>
       <c r="B328" t="n">
-        <v>-0.0003462831268661816</v>
+        <v>-2.462303403102007e-05</v>
       </c>
     </row>
     <row r="329">
@@ -3066,7 +3066,7 @@
         <v>163.5</v>
       </c>
       <c r="B329" t="n">
-        <v>-0.0003720724023723592</v>
+        <v>-0.0005487337639661226</v>
       </c>
     </row>
     <row r="330">
@@ -3074,7 +3074,7 @@
         <v>164</v>
       </c>
       <c r="B330" t="n">
-        <v>-0.0008547573398415782</v>
+        <v>-0.0007673823380238226</v>
       </c>
     </row>
     <row r="331">
@@ -3082,7 +3082,7 @@
         <v>164.5</v>
       </c>
       <c r="B331" t="n">
-        <v>0.000814026342806512</v>
+        <v>0.0007709152343373625</v>
       </c>
     </row>
     <row r="332">
@@ -3090,7 +3090,7 @@
         <v>165</v>
       </c>
       <c r="B332" t="n">
-        <v>0.0007403208404908318</v>
+        <v>0.0005487147087316183</v>
       </c>
     </row>
     <row r="333">
@@ -3098,7 +3098,7 @@
         <v>165.5</v>
       </c>
       <c r="B333" t="n">
-        <v>0.0004960957436194475</v>
+        <v>0.0001532736568365003</v>
       </c>
     </row>
     <row r="334">
@@ -3106,7 +3106,7 @@
         <v>166</v>
       </c>
       <c r="B334" t="n">
-        <v>0.0006050615603570026</v>
+        <v>0.0005426782400384527</v>
       </c>
     </row>
     <row r="335">
@@ -3114,7 +3114,7 @@
         <v>166.5</v>
       </c>
       <c r="B335" t="n">
-        <v>-0.0008554971363751865</v>
+        <v>-0.0002287634182126055</v>
       </c>
     </row>
     <row r="336">
@@ -3122,7 +3122,7 @@
         <v>167</v>
       </c>
       <c r="B336" t="n">
-        <v>0.0005893858543911109</v>
+        <v>9.270471335641949e-05</v>
       </c>
     </row>
     <row r="337">
@@ -3130,7 +3130,7 @@
         <v>167.5</v>
       </c>
       <c r="B337" t="n">
-        <v>7.345640745928037e-05</v>
+        <v>0.0007255268168573117</v>
       </c>
     </row>
     <row r="338">
@@ -3138,7 +3138,7 @@
         <v>168</v>
       </c>
       <c r="B338" t="n">
-        <v>-0.0005441686580908681</v>
+        <v>-0.0001645040547718141</v>
       </c>
     </row>
     <row r="339">
@@ -3146,7 +3146,7 @@
         <v>168.5</v>
       </c>
       <c r="B339" t="n">
-        <v>0.0001018262407136722</v>
+        <v>0.0001966355432623438</v>
       </c>
     </row>
     <row r="340">
@@ -3154,7 +3154,7 @@
         <v>169</v>
       </c>
       <c r="B340" t="n">
-        <v>-0.0001965288437603984</v>
+        <v>0.0008620618300723742</v>
       </c>
     </row>
     <row r="341">
@@ -3162,7 +3162,7 @@
         <v>169.5</v>
       </c>
       <c r="B341" t="n">
-        <v>0.0002548066663529042</v>
+        <v>-0.0001278286052356023</v>
       </c>
     </row>
     <row r="342">
@@ -3170,7 +3170,7 @@
         <v>170</v>
       </c>
       <c r="B342" t="n">
-        <v>-0.0006805628661456165</v>
+        <v>-0.0008539482033116447</v>
       </c>
     </row>
     <row r="343">
@@ -3178,7 +3178,7 @@
         <v>170.5</v>
       </c>
       <c r="B343" t="n">
-        <v>0.0005952680185454374</v>
+        <v>0.000743394996897995</v>
       </c>
     </row>
     <row r="344">
@@ -3186,7 +3186,7 @@
         <v>171</v>
       </c>
       <c r="B344" t="n">
-        <v>-5.724437334858422e-05</v>
+        <v>-0.0008607131122164664</v>
       </c>
     </row>
     <row r="345">
@@ -3194,7 +3194,7 @@
         <v>171.5</v>
       </c>
       <c r="B345" t="n">
-        <v>-0.0006121620529399236</v>
+        <v>-0.0004059384078134876</v>
       </c>
     </row>
     <row r="346">
@@ -3202,7 +3202,7 @@
         <v>172</v>
       </c>
       <c r="B346" t="n">
-        <v>0.0007544807487725797</v>
+        <v>0.0008255892177469884</v>
       </c>
     </row>
     <row r="347">
@@ -3210,7 +3210,7 @@
         <v>172.5</v>
       </c>
       <c r="B347" t="n">
-        <v>-0.0007385850758492702</v>
+        <v>-0.0004279640044151644</v>
       </c>
     </row>
     <row r="348">
@@ -3218,7 +3218,7 @@
         <v>173</v>
       </c>
       <c r="B348" t="n">
-        <v>-0.0006100397981535354</v>
+        <v>-0.0006990755257359696</v>
       </c>
     </row>
     <row r="349">
@@ -3226,7 +3226,7 @@
         <v>173.5</v>
       </c>
       <c r="B349" t="n">
-        <v>-0.0001116795281919033</v>
+        <v>0.0008096605238064278</v>
       </c>
     </row>
     <row r="350">
@@ -3234,7 +3234,7 @@
         <v>174</v>
       </c>
       <c r="B350" t="n">
-        <v>0.000611224509020927</v>
+        <v>-0.0003397248676563625</v>
       </c>
     </row>
     <row r="351">
@@ -3242,7 +3242,7 @@
         <v>174.5</v>
       </c>
       <c r="B351" t="n">
-        <v>0.0006691402210455453</v>
+        <v>-0.0005145227887722565</v>
       </c>
     </row>
     <row r="352">
@@ -3250,7 +3250,7 @@
         <v>175</v>
       </c>
       <c r="B352" t="n">
-        <v>0.0005323893135115493</v>
+        <v>0.0003949051124014362</v>
       </c>
     </row>
     <row r="353">
@@ -3258,7 +3258,7 @@
         <v>175.5</v>
       </c>
       <c r="B353" t="n">
-        <v>0.0003000350970155846</v>
+        <v>0.0007372162428824163</v>
       </c>
     </row>
     <row r="354">
@@ -3266,7 +3266,7 @@
         <v>176</v>
       </c>
       <c r="B354" t="n">
-        <v>-9.459221306470681e-05</v>
+        <v>0.0001773099760270501</v>
       </c>
     </row>
     <row r="355">
@@ -3274,7 +3274,7 @@
         <v>176.5</v>
       </c>
       <c r="B355" t="n">
-        <v>0.0001491568420609763</v>
+        <v>3.550048099685459e-05</v>
       </c>
     </row>
     <row r="356">
@@ -3282,7 +3282,7 @@
         <v>177</v>
       </c>
       <c r="B356" t="n">
-        <v>-0.0004535683205901128</v>
+        <v>-0.0008266243306854693</v>
       </c>
     </row>
     <row r="357">
@@ -3290,7 +3290,7 @@
         <v>177.5</v>
       </c>
       <c r="B357" t="n">
-        <v>-0.0007918452806695835</v>
+        <v>0.0001919430869709236</v>
       </c>
     </row>
     <row r="358">
@@ -3298,7 +3298,7 @@
         <v>178</v>
       </c>
       <c r="B358" t="n">
-        <v>-0.0003853034682530721</v>
+        <v>-3.035899038098814e-05</v>
       </c>
     </row>
     <row r="359">
@@ -3306,7 +3306,7 @@
         <v>178.5</v>
       </c>
       <c r="B359" t="n">
-        <v>4.057943682095546e-05</v>
+        <v>-4.978692875894787e-05</v>
       </c>
     </row>
     <row r="360">
@@ -3314,7 +3314,7 @@
         <v>179</v>
       </c>
       <c r="B360" t="n">
-        <v>-0.0008155535933785767</v>
+        <v>-0.0007719946864811726</v>
       </c>
     </row>
     <row r="361">
@@ -3322,7 +3322,7 @@
         <v>179.5</v>
       </c>
       <c r="B361" t="n">
-        <v>0.0006951566246274457</v>
+        <v>0.0003582738351152072</v>
       </c>
     </row>
     <row r="362">
@@ -3330,7 +3330,7 @@
         <v>180</v>
       </c>
       <c r="B362" t="n">
-        <v>-5.140331254443286e-05</v>
+        <v>-0.0004538375126429851</v>
       </c>
     </row>
   </sheetData>

</xml_diff>